<commit_message>
Change road and mind map
</commit_message>
<xml_diff>
--- a/docs/roadmap.xlsx
+++ b/docs/roadmap.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MarioSlim\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\mind-maps\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>Итерация</t>
   </si>
@@ -65,109 +65,79 @@
     <t>Mind-maps</t>
   </si>
   <si>
-    <t>Центральный прямоугольник, прямоугольники первого уровня</t>
-  </si>
-  <si>
-    <t>В середине экрана расположен прямоугольник, вокруг него другие прямоугольники.</t>
-  </si>
-  <si>
-    <t>Пользователь добавляет центральный прямоугольник при нажатии на клавишу, добавляет прямоугольники первого уровня таким же способом</t>
-  </si>
-  <si>
-    <t xml:space="preserve">• Рисования прямоугольников 
-• Обработка событий, при которых прямоугольники рисуются.
+    <t>Показана структура всей MindMap (заранее задана в коде)</t>
+  </si>
+  <si>
+    <t>Навигация по элементам при помощи стрелок клавиатуры.
+Выделение (outline)  текущего элемента.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> верстка страницы: canvas + элементы управления. canvas на всю область просмотра (кроме верхней панель с кнопками). При старте страницы отрисовывается заранее заданная структура.
+Обрабатывать события нажатия стрелок для показа текущего элемента. 
 </t>
   </si>
   <si>
-    <t>Связь прямоугольников первого уровня</t>
-  </si>
-  <si>
-    <t>В середине экрана центральный прямоугольник, прямоугольники первого уровня связаны линями</t>
-  </si>
-  <si>
-    <t>Пользователь может связывать центральный прямоугольник с прямоугольниками первого уровня</t>
-  </si>
-  <si>
-    <t xml:space="preserve">• Рисование линии.
-• Рисование линии, которая связывает два прямоугольника между собой. </t>
-  </si>
-  <si>
-    <t>Добавление прямоугольников следующих уровней.</t>
-  </si>
-  <si>
-    <t>Пользователь видить связанную сеть</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Возможность создания многоуровневой сети. Выбор следующего прямоугольника, от которого рисовать следующии уровни. </t>
-  </si>
-  <si>
-    <t>• Рисование дополнительных уровней 
-• Обработка события, при котором пользователь выбирает главный прямоугольник.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Добавление текста в прямоугольники. </t>
-  </si>
-  <si>
-    <t>Пользователь может записывать информацию в прямоугольник, при двойном клике на прямоугольник.</t>
-  </si>
-  <si>
-    <t>Возможность чтения</t>
-  </si>
-  <si>
-    <t>Добавление фичей</t>
-  </si>
-  <si>
-    <t>Устранение багов и недочетов. Работа над оформлением.</t>
-  </si>
-  <si>
-    <t>Фигуры могут принимать различные цвета</t>
-  </si>
-  <si>
-    <t>Пользователь может менять цвет фигур, текста</t>
-  </si>
-  <si>
-    <t>• Редактирования цвета
-• Утранение багов, недочетов</t>
-  </si>
-  <si>
-    <t>Фичи</t>
-  </si>
-  <si>
-    <t>Комбинация клавиш</t>
-  </si>
-  <si>
-    <t>Стандартные клавиши копирования, вставки(Ctrl C, Ctrl V).</t>
-  </si>
-  <si>
-    <t>Копирование темы</t>
-  </si>
-  <si>
-    <t>Создание темы в какой либо стороне</t>
-  </si>
-  <si>
-    <t>Редактирование темы</t>
-  </si>
-  <si>
-    <t>Создание блока</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Для создания блока используется двойной щелчок левой кнопкой мыши по области. Или shift + enter для создания дочернего элемента блока</t>
-  </si>
-  <si>
-    <t>Для создания блока слева(справа, сверху, снизу) shift + стрелка влево(вправо, вверх, вниз)</t>
-  </si>
-  <si>
-    <t>Нажать Enter на блоке, текст сохранится. Ширина и высота блока зависит от текста, если текст большой то можно переместить текст на новую строку ctrl + enter.</t>
-  </si>
-  <si>
-    <t>У пользователя есть шаблоны, различные фигуры. Появление картинок</t>
-  </si>
-  <si>
-    <t>Пользователь может выбирать шаблоны, и фигуры. Вставлять картинки</t>
-  </si>
-  <si>
-    <t>• Создание шаблонов, фигур, добавление картинок
-• Добавление дополнительных горячих клавиш</t>
+    <t>Обрабатывать события клавиатуры для добавления подэлемента. Новый элемент создаётся со стандартным текстом. удаление элемента (или поддерева)</t>
+  </si>
+  <si>
+    <t>При нажатии на клавиши будут добавляться новые подэлементы. Элемент создается со стандартным текстом.</t>
+  </si>
+  <si>
+    <t>Структура MindMap</t>
+  </si>
+  <si>
+    <t>Связи. Редактирование текста. Выделение элемента кликом</t>
+  </si>
+  <si>
+    <t>Связанная карта. Элемент выделяется при помощи клика. Можно писать текст.</t>
+  </si>
+  <si>
+    <t>Пользователь может редактировать текст.</t>
+  </si>
+  <si>
+    <t>Перетаскивание элемента мышкой</t>
+  </si>
+  <si>
+    <t>Выберается элемент и перетаскивается в другое место.</t>
+  </si>
+  <si>
+    <t>Импорт, экспорт карты.</t>
+  </si>
+  <si>
+    <t>Импорт, экспорт.</t>
+  </si>
+  <si>
+    <t>Сохранение карты. Загрузка карты.</t>
+  </si>
+  <si>
+    <t>Сохранять карту, загружать карту.</t>
+  </si>
+  <si>
+    <t>Смена внешнего вида MindMap (+2-3 отображения кроме стандартного). Устранение багов.</t>
+  </si>
+  <si>
+    <t>Устранение багов и недочетов. Дополнительный внешний вид</t>
+  </si>
+  <si>
+    <t>Есть еще 2-3 варианта отображения карты.</t>
+  </si>
+  <si>
+    <t>Выбор карты на свой вкус.</t>
+  </si>
+  <si>
+    <t>Перетаскивание элемента мышкой.</t>
+  </si>
+  <si>
+    <t>Добавлять элементы при нажатии на клавишу Tab.</t>
+  </si>
+  <si>
+    <t>Добавление элементов с помощью клавиатуры</t>
+  </si>
+  <si>
+    <t>Рисование линий. Выделение элемента кликом. Редактирование текста (Двойной клик по элементу или F2) Сохранение по Enter.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Выбирать произвольные элементы, перетаскивать их в другое место. </t>
   </si>
 </sst>
 </file>
@@ -240,7 +210,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -313,65 +283,15 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -383,24 +303,32 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -681,10 +609,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:H19"/>
+  <dimension ref="B1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E7" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12:D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -701,18 +629,18 @@
   <sheetData>
     <row r="1" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:8" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="6"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="11"/>
     </row>
     <row r="3" spans="2:8" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="3" t="s">
@@ -735,7 +663,7 @@
       </c>
     </row>
     <row r="4" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="5" t="s">
         <v>1</v>
       </c>
       <c r="C4" s="1"/>
@@ -746,168 +674,162 @@
       <c r="H4" s="1"/>
     </row>
     <row r="5" spans="2:8" ht="93" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" ht="102.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="D6" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="E6" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" ht="124.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="F5" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="G5" s="11" t="s">
+      <c r="F7" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" ht="211.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="H8" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="H5" s="11" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="2:8" ht="102.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="F6" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="G6" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="H6" s="9" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="2:8" ht="124.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="F7" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="G7" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="H7" s="9" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="8" spans="2:8" ht="112.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="F8" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="G8" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="H8" s="9" t="s">
-        <v>32</v>
-      </c>
     </row>
     <row r="12" spans="2:8" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B12" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="C12" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="D12" s="13"/>
+      <c r="B12" s="12"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
     </row>
     <row r="13" spans="2:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="C13" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="D13" s="16"/>
+      <c r="B13" s="16"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="18"/>
     </row>
     <row r="14" spans="2:8" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="C14" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="D14" s="16"/>
-    </row>
-    <row r="15" spans="2:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="B15" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="C15" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="D15" s="16"/>
+      <c r="B14" s="16"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="18"/>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B15" s="16"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="18"/>
     </row>
     <row r="16" spans="2:8" ht="69" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="C16" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="D16" s="16"/>
+      <c r="B16" s="16"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="18"/>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B17" s="17"/>
-      <c r="C17" s="15"/>
-      <c r="D17" s="16"/>
+      <c r="B17" s="13"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="14"/>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B18" s="17"/>
-      <c r="C18" s="15"/>
-      <c r="D18" s="16"/>
+      <c r="B18" s="13"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="14"/>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B19" s="17"/>
-      <c r="C19" s="15"/>
-      <c r="D19" s="16"/>
+      <c r="B19" s="13"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B20" s="15"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="15"/>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B21" s="15"/>
+      <c r="C21" s="15"/>
+      <c r="D21" s="15"/>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B22" s="15"/>
+      <c r="C22" s="15"/>
+      <c r="D22" s="15"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="C16:D16"/>
+  <mergeCells count="4">
     <mergeCell ref="C17:D17"/>
     <mergeCell ref="C18:D18"/>
     <mergeCell ref="C19:D19"/>
     <mergeCell ref="B2:H2"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C15:D15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
I have traded places the 4 and 5 iteration
</commit_message>
<xml_diff>
--- a/docs/roadmap.xlsx
+++ b/docs/roadmap.xlsx
@@ -287,7 +287,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -319,6 +319,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -328,7 +332,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -609,10 +612,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:H22"/>
+  <dimension ref="B1:I22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -627,19 +630,19 @@
     <col min="8" max="8" width="23.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:8" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="15" t="s">
+    <row r="1" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:9" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="17"/>
-    </row>
-    <row r="3" spans="2:8" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="19"/>
+    </row>
+    <row r="3" spans="2:9" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="s">
         <v>0</v>
       </c>
@@ -662,30 +665,30 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="18">
+      <c r="C4" s="15">
         <v>42904</v>
       </c>
-      <c r="D4" s="18">
+      <c r="D4" s="15">
         <v>42918</v>
       </c>
-      <c r="E4" s="18">
+      <c r="E4" s="15">
         <v>42932</v>
       </c>
-      <c r="F4" s="18">
+      <c r="F4" s="15">
         <v>42946</v>
       </c>
-      <c r="G4" s="18">
+      <c r="G4" s="15">
         <v>42960</v>
       </c>
-      <c r="H4" s="18">
+      <c r="H4" s="15">
         <v>42974</v>
       </c>
     </row>
-    <row r="5" spans="2:8" ht="93" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:9" ht="93" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="6" t="s">
         <v>2</v>
       </c>
@@ -699,16 +702,17 @@
         <v>19</v>
       </c>
       <c r="F5" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5" s="7" t="s">
         <v>22</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>25</v>
       </c>
       <c r="H5" s="7" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="6" spans="2:8" ht="102.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I5" s="9"/>
+    </row>
+    <row r="6" spans="2:9" ht="102.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="6" t="s">
         <v>3</v>
       </c>
@@ -722,16 +726,17 @@
         <v>20</v>
       </c>
       <c r="F6" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G6" s="5" t="s">
         <v>23</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>26</v>
       </c>
       <c r="H6" s="5" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="7" spans="2:8" ht="124.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I6" s="14"/>
+    </row>
+    <row r="7" spans="2:9" ht="124.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="6" t="s">
         <v>4</v>
       </c>
@@ -745,16 +750,17 @@
         <v>21</v>
       </c>
       <c r="F7" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G7" s="5" t="s">
         <v>36</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>27</v>
       </c>
       <c r="H7" s="5" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="8" spans="2:8" ht="211.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I7" s="14"/>
+    </row>
+    <row r="8" spans="2:9" ht="211.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="6" t="s">
         <v>5</v>
       </c>
@@ -768,39 +774,40 @@
         <v>35</v>
       </c>
       <c r="F8" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G8" s="5" t="s">
         <v>32</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>24</v>
       </c>
       <c r="H8" s="5" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="12" spans="2:8" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="I8" s="14"/>
+    </row>
+    <row r="12" spans="2:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
       <c r="D12" s="8"/>
     </row>
-    <row r="13" spans="2:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:9" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="11"/>
       <c r="C13" s="12"/>
       <c r="D13" s="12"/>
       <c r="E13" s="13"/>
     </row>
-    <row r="14" spans="2:8" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:9" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="11"/>
       <c r="C14" s="12"/>
       <c r="D14" s="12"/>
       <c r="E14" s="13"/>
     </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B15" s="11"/>
       <c r="C15" s="12"/>
       <c r="D15" s="12"/>
       <c r="E15" s="13"/>
     </row>
-    <row r="16" spans="2:8" ht="69" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:9" ht="69" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="11"/>
       <c r="C16" s="12"/>
       <c r="D16" s="12"/>
@@ -808,18 +815,18 @@
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" s="9"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="16"/>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="9"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
+      <c r="C18" s="16"/>
+      <c r="D18" s="16"/>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" s="9"/>
-      <c r="C19" s="14"/>
-      <c r="D19" s="14"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="16"/>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" s="10"/>

</xml_diff>